<commit_message>
fix: Correct comment in addSeccionesAndDocentesBulk method and improve modal overflow handling
</commit_message>
<xml_diff>
--- a/public/plantilla_excel.xlsx
+++ b/public/plantilla_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braya\Documents\nextjs\asignacion-de-horario-web\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1137E632-E076-430C-B8FB-DC246A05149B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35E96B9-A47A-4301-9572-908D54C87E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{61FC1DF7-9949-4AF0-ABDD-4959043D061E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
   <si>
     <t>diaSemana</t>
   </si>
@@ -48,13 +48,40 @@
   </si>
   <si>
     <t>tipoRestriccion</t>
+  </si>
+  <si>
+    <t>jueves</t>
+  </si>
+  <si>
+    <t>disponible</t>
+  </si>
+  <si>
+    <t>lunes</t>
+  </si>
+  <si>
+    <t>martes</t>
+  </si>
+  <si>
+    <t>viernes</t>
+  </si>
+  <si>
+    <t>bloqueado</t>
+  </si>
+  <si>
+    <t>miercoles</t>
+  </si>
+  <si>
+    <t>sabado</t>
+  </si>
+  <si>
+    <t>Tipos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,16 +89,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFEE0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -79,12 +152,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF42CE1-4E2B-4931-BA52-B0038D71885D}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,24 +541,291 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D19" xr:uid="{02CB09A9-BE18-4BBB-A7F1-699FE7B81729}">
+      <formula1>$G$1:$H$1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>